<commit_message>
Adds Endotherm to KillRatePreyMassExponent in RevisedPredation
</commit_message>
<xml_diff>
--- a/probeWNewEndos_Error.xlsx
+++ b/probeWNewEndos_Error.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MadingleyProbe_EctoEndoForage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B581327-EC29-496F-B8F3-0A1ECB78350B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE214F5-1BAC-4FBC-8BD9-626B01F276ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{1E20459E-22FE-495B-B983-F02A2B4BFEAE}"/>
+    <workbookView xWindow="30825" yWindow="840" windowWidth="23085" windowHeight="17085" xr2:uid="{1E20459E-22FE-495B-B983-F02A2B4BFEAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>_SpecificPredatorKillRateConstant</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>Set within a method in Revised Predation; line 587</t>
+  </si>
+  <si>
+    <t>_KillRatePreyMassExponent</t>
+  </si>
+  <si>
+    <t>Predation.RevisedPredation.KillRatePreyMassExponent</t>
+  </si>
+  <si>
+    <t>Predation.RevisedPredation.Endotherm.KillRatePreyMassExponent</t>
   </si>
 </sst>
 </file>
@@ -224,19 +233,19 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -552,13 +561,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7367503-B662-4804-9B4A-367946DB9EC2}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
+      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,39 +582,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
@@ -622,8 +631,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="7"/>
       <c r="D3" t="s">
         <v>2</v>
       </c>
@@ -638,8 +647,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="5"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="7"/>
       <c r="D4" t="s">
         <v>3</v>
       </c>
@@ -654,12 +663,12 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="7"/>
       <c r="C6" t="s">
         <v>4</v>
       </c>
@@ -677,8 +686,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="7"/>
       <c r="D7" t="s">
         <v>6</v>
       </c>
@@ -693,16 +702,16 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="5"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="5"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="8"/>
+      <c r="B10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
@@ -711,10 +720,10 @@
       <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="5" t="s">
         <v>30</v>
       </c>
       <c r="H10">
@@ -722,15 +731,15 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="5"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="7"/>
       <c r="D11" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="5" t="s">
         <v>31</v>
       </c>
       <c r="H11">
@@ -738,22 +747,22 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="5"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="5"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="7"/>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="5" t="s">
         <v>36</v>
       </c>
       <c r="H13">
@@ -761,15 +770,15 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="7"/>
       <c r="D14" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="5" t="s">
         <v>38</v>
       </c>
       <c r="H14">
@@ -777,12 +786,12 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="5"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="7"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="8"/>
+      <c r="B16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
@@ -791,33 +800,33 @@
       <c r="D16" t="s">
         <v>0</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="3"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="8"/>
+      <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3"/>
-      <c r="G19" s="4"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="2"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C20" t="s">
@@ -834,7 +843,21 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H22">
+        <v>-8.8319999999999996E-2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>